<commit_message>
Points can be read
</commit_message>
<xml_diff>
--- a/points.xlsx
+++ b/points.xlsx
@@ -2,46 +2,27 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="5760" yWindow="0" windowWidth="17280" windowHeight="8964" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1" refMode="A1" iterate="0" iterateCount="100" iterateDelta="0.0001"/>
+  <calcPr calcId="0" fullCalcOnLoad="1" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="4">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <charset val="1"/>
       <family val="2"/>
       <color rgb="FF000000"/>
       <sz val="11"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <charset val="238"/>
-      <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <charset val="238"/>
-      <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <charset val="238"/>
-      <family val="0"/>
-      <sz val="10"/>
     </font>
   </fonts>
   <fills count="2">
@@ -61,33 +42,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="2" builtinId="6"/>
-    <cellStyle name="Currency" xfId="3" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Percent" xfId="5" builtinId="5"/>
+  <cellStyles count="1">
+    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -444,31 +409,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr filterMode="0">
+  <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr fitToPage="0"/>
+    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.55078125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.5546875" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" ht="15" customHeight="1" s="1">
-      <c r="A1" s="2" t="inlineStr">
+      <c r="A1" t="inlineStr">
         <is>
           <t>Sedarius</t>
         </is>
       </c>
-      <c r="C1" s="2" t="n">
-        <v>6</v>
+      <c r="C1" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
-  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup orientation="portrait" paperSize="9" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup orientation="portrait" paperSize="9" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added command list, bot now checks if user exists on server and checks if user has points tracked already
</commit_message>
<xml_diff>
--- a/points.xlsx
+++ b/points.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="5760" yWindow="0" windowWidth="17280" windowHeight="8964" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" state="visible" r:id="rId1"/>
@@ -45,8 +45,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -416,12 +415,12 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D5" sqref="A3:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="8.5546875" defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" ht="15" customHeight="1" s="1">
+    <row r="1" ht="15" customHeight="1">
       <c r="A1" t="inlineStr">
         <is>
           <t>Sedarius</t>

</xml_diff>

<commit_message>
commands with points work for other users
</commit_message>
<xml_diff>
--- a/points.xlsx
+++ b/points.xlsx
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D5" sqref="A3:D5"/>
@@ -440,6 +440,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Gouenji</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" paperSize="9" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>